<commit_message>
Read excel files into content
</commit_message>
<xml_diff>
--- a/STELARR2/Files/lessons.xlsx
+++ b/STELARR2/Files/lessons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janle\source\repos\lms-stelarr\STELARR2\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69249CC3-45B6-40AA-A499-09BFC0AC6AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED1F88C-EB5A-4989-A6D1-047ABC6FE6EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6100" yWindow="3250" windowWidth="28800" windowHeight="15370" xr2:uid="{4E17EF1E-3C40-4A27-B831-1D6513E14897}"/>
   </bookViews>
@@ -35,15 +35,111 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Math is fun</t>
-  </si>
-  <si>
-    <t>Reading is more fun</t>
-  </si>
-  <si>
-    <t>Music is the best</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>Numbers</t>
+  </si>
+  <si>
+    <t>Letters</t>
+  </si>
+  <si>
+    <t>Words</t>
+  </si>
+  <si>
+    <t>Shapes</t>
+  </si>
+  <si>
+    <t>Colors</t>
+  </si>
+  <si>
+    <t>0, zero, ze-ro</t>
+  </si>
+  <si>
+    <t>Addition,1 + 1 = 2,1 + 2 = 3,1 + 3 = 4</t>
+  </si>
+  <si>
+    <t>A,Ant</t>
+  </si>
+  <si>
+    <t>1, one, wun</t>
+  </si>
+  <si>
+    <t>Commutative Property,2 + 1 = 1 + 2 = 3</t>
+  </si>
+  <si>
+    <t>B,Bird</t>
+  </si>
+  <si>
+    <t>2, two, tu</t>
+  </si>
+  <si>
+    <t>Identity Property,3 + 0 = 3,0 + 5 = 5</t>
+  </si>
+  <si>
+    <t>C,Cat</t>
+  </si>
+  <si>
+    <t>3, three, three</t>
+  </si>
+  <si>
+    <t>Associative Property,(2 + 1) + 3 = 2 + (1 + 3) = 6</t>
+  </si>
+  <si>
+    <t>D,Dog</t>
+  </si>
+  <si>
+    <t>4, four, for</t>
+  </si>
+  <si>
+    <t>Examples,4 + 4 = ?, 5 + 1 = ?,6 + 0 = ?</t>
+  </si>
+  <si>
+    <t>E,Elephant</t>
+  </si>
+  <si>
+    <t>5, five, fayv</t>
+  </si>
+  <si>
+    <t>Subtraction,3 - 2 = 1,5 - 2 = 3,2 -2 = 0</t>
+  </si>
+  <si>
+    <t>F,Frog</t>
+  </si>
+  <si>
+    <t>6, six, six</t>
+  </si>
+  <si>
+    <t>Subtraction,3 - 2 = 1,3 is the minuend,2 is the subtrahend,1 is the difference</t>
+  </si>
+  <si>
+    <t>G,Giraffe</t>
+  </si>
+  <si>
+    <t>7, seven, se-ven</t>
+  </si>
+  <si>
+    <t>Identity Property,5 - 0 = 5, 9 - 0 = 9</t>
+  </si>
+  <si>
+    <t>H,Horse</t>
+  </si>
+  <si>
+    <t>8, eight, eyt</t>
+  </si>
+  <si>
+    <t>I,Iguana</t>
+  </si>
+  <si>
+    <t>9, nine, nayn</t>
+  </si>
+  <si>
+    <t>Examples,3 - 2 = ?,5 - 4 = ?,6 - 0 = ?</t>
+  </si>
+  <si>
+    <t>J,Jellyfish</t>
   </si>
 </sst>
 </file>
@@ -79,8 +175,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,27 +494,147 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{956A866C-3A0A-46CD-B30A-FE6D0CC722CE}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.54296875" defaultRowHeight="29.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="16.453125" defaultRowHeight="64.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.453125" style="1"/>
+    <col min="2" max="2" width="45.54296875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="16.453125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>